<commit_message>
Fix lỗi mã số thuế - bịnối thêm Tên công ty vào
</commit_message>
<xml_diff>
--- a/AutoCompany/Excel/Data.xlsx
+++ b/AutoCompany/Excel/Data.xlsx
@@ -12,12 +12,9 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
-    <sheet name="TINH BINH DINH" sheetId="152" r:id="rId1"/>
-    <sheet name="TINH PHU YEN" sheetId="139" r:id="rId2"/>
-    <sheet name="TINH TAY NINH" sheetId="135" r:id="rId3"/>
-    <sheet name="QUAN 2" sheetId="115" r:id="rId4"/>
-    <sheet name="TINH LAM DONG" sheetId="113" r:id="rId5"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId6"/>
+    <sheet name="TINH BINH DINH" sheetId="26" r:id="rId1"/>
+    <sheet name="HUYEN VINH THANH" sheetId="25" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -29,27 +26,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>22/04/2021</t>
+    <t>CÔNG TY TNHH VẬN TẢI TUẤN MINH BÌNH ĐỊNH</t>
   </si>
   <si>
-    <t>CÔNG TY TNHH LAMVIEN DALAT</t>
+    <t>Lô 15-16 Khu Đô thị An Phú Thịnh, Phường Đống Đa, Thành phố Quy Nhơn, Tỉnh Bình Định</t>
   </si>
   <si>
-    <t>Thôn 1, Xã Lộc Ngãi, Huyện Bảo Lâm, Tỉnh Lâm Đồng</t>
+    <t>Nguyễn Quy Khoa</t>
   </si>
   <si>
-    <t>NGUYỄN VĂN VIÊN</t>
+    <t>CÔNG TY TNHH THƯƠNG MẠI - TỔNG HỢP BÌNH VƯƠNG</t>
   </si>
   <si>
-    <t>CÔNG TY TNHH NĂNG LƯỢNG CAMELLIA</t>
+    <t>Số 295 Nguyễn Thị Minh Khai, Phường Nguyễn Văn Cừ, Thành phố Quy Nhơn, Tỉnh Bình Định</t>
   </si>
   <si>
-    <t>Thôn 4, Xã Ma Đa Guôi, Huyện Đạ Huoai, Tỉnh Lâm Đồng</t>
-  </si>
-  <si>
-    <t>Hoàng Lan Chi</t>
+    <t>Bùi Quốc Thắng</t>
   </si>
 </sst>
 </file>
@@ -368,12 +362,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>4101598873</v>
+      </c>
+      <c r="B1" s="1">
+        <v>44414</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1">
+        <v>965972999</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>4101598880</v>
+      </c>
+      <c r="B2" s="1">
+        <v>44414</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <v>963555405</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -392,86 +427,6 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="16.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>5801462252</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1">
-        <v>979269067</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>5801462277</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2">
-        <v>383809916</v>
-      </c>
-      <c r="F2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B24:B50"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">

</xml_diff>